<commit_message>
DDR_A length matching done
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DDR_A" sheetId="1" state="visible" r:id="rId1"/>
@@ -461,18 +461,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.984375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.2890625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="29.18" customWidth="1" style="2" min="1" max="1"/>
     <col width="19.72" customWidth="1" style="2" min="2" max="2"/>
     <col width="6.11" customWidth="1" style="2" min="3" max="3"/>
-    <col width="15.56" customWidth="1" style="2" min="4" max="4"/>
+    <col width="16.94" customWidth="1" style="2" min="4" max="4"/>
     <col width="15.14" customWidth="1" style="2" min="5" max="5"/>
     <col width="13.89" customWidth="1" style="2" min="6" max="6"/>
     <col width="13.19" customWidth="1" style="2" min="7" max="7"/>
@@ -553,12 +553,12 @@
     <row r="2" ht="13.5" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA0_A</t>
+          <t>DRAM_D07_A</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -570,39 +570,39 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>10.48</v>
+        <v>20.99</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>10.88</v>
+        <v>21.39</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>72.93000000000001</v>
+        <v>144.85</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>100</v>
+        <v>51.4</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>177.53</v>
+        <v>200.85</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA1_A</t>
+          <t>DRAM_D05_A</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -614,39 +614,39 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>10.52</v>
+        <v>19.98</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>10.92</v>
+        <v>20.38</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>73.19</v>
+        <v>138.13</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0</v>
+        <v>58.1</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>77.78999999999999</v>
+        <v>200.83</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA2_A</t>
+          <t>DRAM_D01_A</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -658,39 +658,39 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>16.7</v>
+        <v>22.34</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>17.1</v>
+        <v>22.74</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>116.96</v>
+        <v>153.17</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>121.56</v>
+        <v>200.77</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA3_A</t>
+          <t>DRAM_D06_A</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -702,39 +702,39 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>18.18</v>
+        <v>18.85</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>18.58</v>
+        <v>19.25</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>127.51</v>
+        <v>131.54</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>132.11</v>
+        <v>200.74</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA4_A</t>
+          <t>DRAM_D00_A</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -746,39 +746,39 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>17.51</v>
+        <v>22.13</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>17.91</v>
+        <v>22.53</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>122.65</v>
+        <v>153.41</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0</v>
+        <v>42.7</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>127.25</v>
+        <v>200.71</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA5_A</t>
+          <t>DRAM_D03_A</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -790,28 +790,28 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>17.89</v>
+        <v>20.84</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>18.29</v>
+        <v>21.24</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>125.47</v>
+        <v>144.33</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0</v>
+        <v>51.7</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>130.07</v>
+        <v>200.63</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">
@@ -822,7 +822,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D00_A</t>
+          <t>DRAM_D04_A</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -834,28 +834,28 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>19.96</v>
+        <v>19.62</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>20.36</v>
+        <v>20.02</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>137.01</v>
+        <v>136.13</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0</v>
+        <v>59.9</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>141.61</v>
+        <v>200.63</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
@@ -866,7 +866,7 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D01_A</t>
+          <t>DRAM_DMI0_A</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -878,28 +878,28 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>22.51</v>
+        <v>20.16</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>22.91</v>
+        <v>20.56</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>154.81</v>
+        <v>138.62</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0</v>
+        <v>57.2</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>159.41</v>
+        <v>200.42</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
@@ -922,39 +922,39 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>18.92</v>
+        <v>20.36</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>19.32</v>
+        <v>20.76</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>130.89</v>
+        <v>141.08</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0</v>
+        <v>54.6</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>135.49</v>
+        <v>200.28</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="3">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 0 – DQS</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D03_A</t>
+          <t>DRAM_DQS0_A_P</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -962,43 +962,43 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>15.92</v>
+        <v>17.8</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>16.32</v>
+        <v>20.2</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>109.67</v>
+        <v>104.27</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>114.27</v>
+        <v>199.27</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="3">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 0 – DQS</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D04_A</t>
+          <t>DRAM_DQS0_A_N</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1006,43 +1006,43 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>14.69</v>
+        <v>17.8</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>15.09</v>
+        <v>20.2</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>100.73</v>
+        <v>104.16</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>0</v>
+        <v>58.9</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>105.33</v>
+        <v>199.06</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="3">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D05_A</t>
+          <t>DRAM_CA3_A</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1054,39 +1054,39 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>14.04</v>
+        <v>18.18</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>14.44</v>
+        <v>18.58</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>96.06</v>
+        <v>127.51</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>0</v>
+        <v>59.7</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>100.66</v>
+        <v>191.81</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="3">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D06_A</t>
+          <t>DRAM_CA0_A</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1098,39 +1098,39 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>15.86</v>
+        <v>21.03</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>16.26</v>
+        <v>21.43</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>110.44</v>
+        <v>147.57</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>0</v>
+        <v>39.6</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>115.04</v>
+        <v>191.77</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D07_A</t>
+          <t>DRAM_CKE0_A</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1138,398 +1138,914 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, In2.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>17.39</v>
+        <v>19.86</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>17.79</v>
+        <v>21.26</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>119.42</v>
+        <v>138.74</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>4.6</v>
+        <v>20.3</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>0</v>
+        <v>51.2</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>0</v>
+        <v>-18.48</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>124.02</v>
+        <v>191.76</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D08_A</t>
+          <t>DRAM_CA2_A</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>10.32</v>
+        <v>18.87</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>10.32</v>
+        <v>19.27</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>60.35</v>
+        <v>132.31</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>0</v>
+        <v>54.8</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>60.35</v>
+        <v>191.71</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" s="3">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D09_A</t>
+          <t>DRAM_CA5_A</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>9.02</v>
+        <v>22.08</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>9.02</v>
+        <v>22.48</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>52.73</v>
+        <v>155.11</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>52.73</v>
+        <v>191.71</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" s="3">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D10_A</t>
+          <t>DRAM_CKE1_A</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>9.31</v>
+        <v>21.45</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>9.31</v>
+        <v>22.85</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>54.5</v>
+        <v>149.96</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>0</v>
+        <v>20.3</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0</v>
+        <v>-18.48</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>54.5</v>
+        <v>191.68</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" s="3">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D11_A</t>
+          <t>~{DRAM_CS1_A}</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>8.5</v>
+        <v>20.35</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>8.5</v>
+        <v>20.75</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>49.67</v>
+        <v>142.76</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>0</v>
+        <v>44.2</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>49.67</v>
+        <v>191.56</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D12_A</t>
+          <t>DRAM_CA1_A</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>8.300000000000001</v>
+        <v>22.47</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>8.300000000000001</v>
+        <v>22.87</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>48.5</v>
+        <v>157.8</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>48.5</v>
+        <v>191.5</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" s="3">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D13_A</t>
+          <t>DRAM_CA4_A</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>12.05</v>
+        <v>21.8</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>12.05</v>
+        <v>22.2</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>70.59999999999999</v>
+        <v>153.03</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>0</v>
+        <v>33.8</v>
       </c>
       <c r="K21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>70.59999999999999</v>
+        <v>191.43</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D14_A</t>
+          <t>~{DRAM_CS0_A}</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>12.39</v>
+        <v>21.49</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>12.39</v>
+        <v>21.89</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>72.54000000000001</v>
+        <v>150.82</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>0</v>
+        <v>35.9</v>
       </c>
       <c r="K22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>72.54000000000001</v>
+        <v>191.32</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
       <c r="A23" s="2" t="inlineStr">
         <is>
+          <t>Clock</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CK_A_N</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>19.7</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>115.37</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>-3.35</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>189.22</v>
+      </c>
+    </row>
+    <row r="24" ht="13.5" customHeight="1" s="3">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Clock</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CK_A_P</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>19.68</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>22.08</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>115.12</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>41.1</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>-3.35</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>188.87</v>
+      </c>
+    </row>
+    <row r="25" ht="13.5" customHeight="1" s="3">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
           <t>Byte Lane 1</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D13_A</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>16.38</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>16.38</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>95.88</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>48.8</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>144.68</v>
+      </c>
+    </row>
+    <row r="26" ht="13.5" customHeight="1" s="3">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D12_A</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>17.86</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>17.86</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>104.35</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>40.3</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>144.65</v>
+      </c>
+    </row>
+    <row r="27" ht="13.5" customHeight="1" s="3">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D08_A</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>17.06</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>17.06</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>144.6</v>
+      </c>
+    </row>
+    <row r="28" ht="13.5" customHeight="1" s="3">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D11_A</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>16.66</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>16.66</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>97.29000000000001</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>47.2</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>144.49</v>
+      </c>
+    </row>
+    <row r="29" ht="13.5" customHeight="1" s="3">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1 – DQS</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_DQS1_A_P</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>10.22</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>12.62</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>59.84</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>144.44</v>
+      </c>
+    </row>
+    <row r="30" ht="13.5" customHeight="1" s="3">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D09_A</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>16.15</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>16.15</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>94.31999999999999</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>50.1</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>144.42</v>
+      </c>
+    </row>
+    <row r="31" ht="13.5" customHeight="1" s="3">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1 – DQS</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_DQS1_A_N</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>12.84</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>61.17</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>47.2</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>144.37</v>
+      </c>
+    </row>
+    <row r="32" ht="13.5" customHeight="1" s="3">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_DMI1_A</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>85.77</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>58.6</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>144.37</v>
+      </c>
+    </row>
+    <row r="33" ht="13.5" customHeight="1" s="3">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D10_A</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>16.77</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>16.77</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>98.01000000000001</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="n">
+        <v>144.21</v>
+      </c>
+    </row>
+    <row r="34" ht="13.5" customHeight="1" s="3">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D14_A</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>85.73999999999999</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>58.4</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>144.14</v>
+      </c>
+    </row>
+    <row r="35" ht="13.5" customHeight="1" s="3">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>DRAM_D15_A</t>
         </is>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="C35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
         <is>
           <t>F.Cu</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>14.64</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>14.64</v>
-      </c>
-      <c r="H23" s="2" t="n">
-        <v>85.65000000000001</v>
-      </c>
-      <c r="I23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2" t="n">
-        <v>85.65000000000001</v>
-      </c>
-    </row>
-    <row r="24" ht="13.5" customHeight="1" s="3"/>
-    <row r="25" ht="13.5" customHeight="1" s="3"/>
-    <row r="26" ht="13.5" customHeight="1" s="3"/>
-    <row r="27" ht="13.5" customHeight="1" s="3"/>
-    <row r="28" ht="13.5" customHeight="1" s="3"/>
-    <row r="29" ht="13.5" customHeight="1" s="3"/>
-    <row r="30" ht="13.5" customHeight="1" s="3"/>
-    <row r="31" ht="13.5" customHeight="1" s="3"/>
-    <row r="32" ht="13.5" customHeight="1" s="3"/>
-    <row r="33" ht="13.5" customHeight="1" s="3"/>
-    <row r="34" ht="13.5" customHeight="1" s="3"/>
-    <row r="35" ht="13.5" customHeight="1" s="3"/>
+      <c r="E35" s="2" t="n">
+        <v>15.67</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>15.67</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>91.64</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>144.04</v>
+      </c>
+    </row>
     <row r="36" ht="13.5" customHeight="1" s="3"/>
     <row r="37" ht="13.5" customHeight="1" s="3"/>
     <row r="38" ht="13.5" customHeight="1" s="3"/>
@@ -1571,11 +2087,11 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.984375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.2890625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="29.18" customWidth="1" style="2" min="1" max="1"/>
     <col width="19.72" customWidth="1" style="2" min="2" max="2"/>
@@ -1661,12 +2177,12 @@
     <row r="2" ht="13.5" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Clock</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA0_B</t>
+          <t>DRAM_CK_B_N</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -1674,43 +2190,43 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11</v>
+        <v>20.12</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>11.4</v>
+        <v>22.52</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>76.59</v>
+        <v>117.86</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0</v>
+        <v>42.2</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>0</v>
+        <v>-3.35</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>81.19</v>
+        <v>192.71</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Clock</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA1_B</t>
+          <t>DRAM_CK_B_P</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -1718,43 +2234,43 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>11.16</v>
+        <v>20.14</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>11.56</v>
+        <v>22.54</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>77.73</v>
+        <v>117.85</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0</v>
+        <v>41.8</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0</v>
+        <v>-3.35</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>82.33</v>
+        <v>192.3</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 1 – DQS</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA2_B</t>
+          <t>DRAM_DQS1_B_N</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -1762,43 +2278,43 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>18.18</v>
+        <v>18.65</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>18.58</v>
+        <v>21.05</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>127.41</v>
+        <v>109.24</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>132.01</v>
+        <v>200.24</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 1 – DQS</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA3_B</t>
+          <t>DRAM_DQS1_B_P</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -1806,43 +2322,43 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>17.62</v>
+        <v>18.4</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>18.02</v>
+        <v>20.8</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>123.45</v>
+        <v>107.64</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0</v>
+        <v>55.5</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>128.05</v>
+        <v>199.14</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA4_B</t>
+          <t>DRAM_D09_B</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -1854,39 +2370,39 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>19.19</v>
+        <v>22.8</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>19.59</v>
+        <v>23.2</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>134.58</v>
+        <v>158.55</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0</v>
+        <v>51.3</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>139.18</v>
+        <v>214.45</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA5_B</t>
+          <t>DRAM_D08_B</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -1898,113 +2414,1261 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>21.16</v>
+        <v>20.1</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>21.56</v>
+        <v>20.5</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>147.93</v>
+        <v>139.91</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0</v>
+        <v>60.2</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>152.53</v>
+        <v>204.71</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">
-      <c r="C8" s="2" t="n"/>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_DMI1_B</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>18.27</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>18.67</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>127.35</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>53.1</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>185.05</v>
+      </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
-      <c r="C9" s="2" t="n"/>
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D15_B</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>19.71</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>20.11</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>135.84</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>184.64</v>
+      </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
-      <c r="C10" s="2" t="n"/>
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D11_B</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>16.87</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>17.27</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>115.84</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>178.44</v>
+      </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="3">
-      <c r="C11" s="2" t="n"/>
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D13_B</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>16.21</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>16.61</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>110.75</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>173.45</v>
+      </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="3">
-      <c r="C12" s="2" t="n"/>
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D10_B</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>17.16</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>17.56</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>116.78</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>48.8</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>170.18</v>
+      </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="3">
-      <c r="C13" s="2" t="n"/>
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D12_B</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>15.23</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>15.63</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>103.8</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>59.1</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>167.5</v>
+      </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="3">
-      <c r="C14" s="2" t="n"/>
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 1</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D14_B</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>16.06</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>16.46</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>111.69</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>166.29</v>
+      </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
-      <c r="C15" s="2" t="n"/>
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0 – DQS</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_DQS0_B_N</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>64.41</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>149.01</v>
+      </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
-      <c r="C16" s="2" t="n"/>
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0 – DQS</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_DQS0_B_P</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>64.41</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>149.01</v>
+      </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" s="3">
-      <c r="C17" s="2" t="n"/>
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D07_B</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>13.37</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>13.37</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>78.12</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>126.12</v>
+      </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" s="3">
-      <c r="C18" s="2" t="n"/>
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D05_B</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>11.92</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>11.92</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>69.64</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>119.44</v>
+      </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" s="3">
-      <c r="C19" s="2" t="n"/>
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D04_B</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>65.34</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>118.94</v>
+      </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
-      <c r="C20" s="2" t="n"/>
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D06_B</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>63.15</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>54.7</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>117.85</v>
+      </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" s="3">
-      <c r="C21" s="2" t="n"/>
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_DMI0_B</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>54.25</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>52.8</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>107.05</v>
+      </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
-      <c r="C22" s="2" t="n"/>
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D00_B</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>9.42</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>9.42</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>54.95</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>106.45</v>
+      </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
-      <c r="C23" s="2" t="n"/>
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D02_B</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>50.8</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>54.5</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>105.3</v>
+      </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">
-      <c r="C24" s="2" t="n"/>
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D01_B</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>49.41</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>99.31</v>
+      </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" s="3">
-      <c r="C25" s="2" t="n"/>
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>Byte Lane 0</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_D03_B</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>54.24</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>96.24000000000001</v>
+      </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" s="3">
-      <c r="C26" s="2" t="n"/>
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CKE1_B</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>19.66</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>21.06</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>137.32</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>-18.48</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>190.74</v>
+      </c>
     </row>
     <row r="27" ht="13.5" customHeight="1" s="3">
-      <c r="C27" s="2" t="n"/>
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CA1_B</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>151.65</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>190.65</v>
+      </c>
     </row>
     <row r="28" ht="13.5" customHeight="1" s="3">
-      <c r="C28" s="2" t="n"/>
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CKE0_B</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>19.64</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>21.04</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>137.16</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>-18.48</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>190.58</v>
+      </c>
     </row>
     <row r="29" ht="13.5" customHeight="1" s="3">
-      <c r="C29" s="2" t="n"/>
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CA5_B</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>21.11</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>21.51</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>147.56</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>190.76</v>
+      </c>
     </row>
     <row r="30" ht="13.5" customHeight="1" s="3">
-      <c r="C30" s="2" t="n"/>
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CA4_B</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>21.65</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>22.05</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>151.97</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>190.87</v>
+      </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="3">
-      <c r="C31" s="2" t="n"/>
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CA0_B</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>21.98</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>22.38</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>154.34</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>190.84</v>
+      </c>
     </row>
     <row r="32" ht="13.5" customHeight="1" s="3">
-      <c r="C32" s="2" t="n"/>
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CA3_B</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>18.52</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>18.92</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>129.82</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>190.92</v>
+      </c>
     </row>
     <row r="33" ht="13.5" customHeight="1" s="3">
-      <c r="C33" s="2" t="n"/>
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>~{DRAM_CS0_B}</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>20.84</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>21.24</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>146.22</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="n">
+        <v>190.82</v>
+      </c>
     </row>
     <row r="34" ht="13.5" customHeight="1" s="3">
-      <c r="C34" s="2" t="n"/>
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>~{DRAM_CS1_B}</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>19.76</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>20.16</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>138.57</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>47.7</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>190.87</v>
+      </c>
     </row>
     <row r="35" ht="13.5" customHeight="1" s="3">
-      <c r="C35" s="2" t="n"/>
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>Address, Command and Control</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>DRAM_CA2_B</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, In2.Cu</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>126.82</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>190.92</v>
+      </c>
     </row>
     <row r="36" ht="13.5" customHeight="1" s="3">
       <c r="C36" s="2" t="n"/>
@@ -2087,7 +3751,7 @@
       <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9921875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="13.06" customWidth="1" style="2" min="2" max="2"/>
     <col width="13.06" customWidth="1" style="2" min="10" max="10"/>
@@ -2667,11 +4331,11 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.09375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="14.03" customWidth="1" style="2" min="2" max="2"/>
   </cols>
@@ -2795,7 +4459,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>ENET_TD2</t>
+          <t>ENET_TXC</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -2807,16 +4471,16 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>13.37</v>
+        <v>13.12</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>13.77</v>
+        <v>13.52</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>88.12</v>
+        <v>88.27</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>4.6</v>
@@ -2828,42 +4492,42 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>92.72</v>
+        <v>92.86999999999999</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>RGMII – RX</t>
+          <t>RGMII – TX</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>ENET_RX_CTL</t>
+          <t>ENET_TD2</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>15.35</v>
+        <v>13.37</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>15.35</v>
+        <v>13.77</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>89.90000000000001</v>
+        <v>88.12</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -2872,18 +4536,18 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>89.90000000000001</v>
+        <v>92.72</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>RGMII – RX</t>
+          <t>RGMII – TX</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>ENET_RXC</t>
+          <t>ENET_TD0</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -2895,16 +4559,16 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>13.52</v>
+        <v>13.37</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>13.92</v>
+        <v>13.77</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>84.14</v>
+        <v>86.19</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>4.6</v>
@@ -2916,7 +4580,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>88.73999999999999</v>
+        <v>90.78999999999999</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="3">
@@ -2927,7 +4591,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>ENET_RD3</t>
+          <t>ENET_RX_CTL</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -2939,16 +4603,16 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>14.78</v>
+        <v>15.35</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>14.78</v>
+        <v>15.35</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>86.43000000000001</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>0</v>
@@ -2960,18 +4624,18 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>86.43000000000001</v>
+        <v>89.90000000000001</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>RGMII – TX</t>
+          <t>RGMII – RX</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>ENET_TD1</t>
+          <t>ENET_RXC</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -2983,16 +4647,16 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>12.93</v>
+        <v>13.7</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>13.33</v>
+        <v>14.1</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>81.77</v>
+        <v>85.15000000000001</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>4.6</v>
@@ -3004,42 +4668,42 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>86.36999999999999</v>
+        <v>89.75</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="3">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>RGMII – RX</t>
+          <t>RGMII – TX</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>ENET_RD2</t>
+          <t>ENET_TX_CTL</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>13.77</v>
+        <v>12.4</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>13.77</v>
+        <v>12.8</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>80.51000000000001</v>
+        <v>81.98</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>0</v>
@@ -3048,7 +4712,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>80.51000000000001</v>
+        <v>86.58</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="3">
@@ -3059,31 +4723,31 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>ENET_RD1</t>
+          <t>ENET_RD3</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>12.54</v>
+        <v>14.78</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>12.94</v>
+        <v>14.78</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>74.45999999999999</v>
+        <v>86.43000000000001</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>0</v>
@@ -3092,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>79.05999999999999</v>
+        <v>86.43000000000001</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="3">
@@ -3103,7 +4767,7 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>ENET_TX_CTL</t>
+          <t>ENET_TD1</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -3115,16 +4779,16 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>12.4</v>
+        <v>12.93</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>12.8</v>
+        <v>13.33</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>81.98</v>
+        <v>81.77</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>4.6</v>
@@ -3136,42 +4800,42 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>86.58</v>
+        <v>86.36999999999999</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="3">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>RGMII – TX</t>
+          <t>RGMII – RX</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>ENET_TD0</t>
+          <t>ENET_RD2</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>13.37</v>
+        <v>13.77</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>13.77</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>86.19</v>
+        <v>80.51000000000001</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>0</v>
@@ -3180,42 +4844,42 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>90.78999999999999</v>
+        <v>80.51000000000001</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="3">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>RGMII – TX</t>
+          <t>RGMII – RX</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>ENET_TXC</t>
+          <t>ENET_RD0</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>13.12</v>
+        <v>13.68</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>13.52</v>
+        <v>13.68</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>88.27</v>
+        <v>80.12</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2" t="n">
         <v>0</v>
@@ -3224,7 +4888,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>92.86999999999999</v>
+        <v>80.12</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="3">
@@ -3235,31 +4899,31 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>ENET_RD0</t>
+          <t>ENET_RD1</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>13.68</v>
+        <v>12.54</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>13.68</v>
+        <v>12.94</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>80.12</v>
+        <v>74.45999999999999</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J13" s="2" t="n">
         <v>0</v>
@@ -3268,7 +4932,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>80.12</v>
+        <v>79.05999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3298,7 +4962,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.25390625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="3">
       <c r="A1" s="2" t="inlineStr">
@@ -3387,16 +5051,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>64.02</v>
+        <v>63.94</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1.2</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>65.22</v>
+        <v>65.14</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>374.94</v>
+        <v>374.49</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>18</v>
@@ -3408,7 +5072,7 @@
         <v>31.57</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>424.51</v>
+        <v>424.06</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="3">
@@ -3431,16 +5095,16 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>66.41</v>
+        <v>66.45999999999999</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>68.81</v>
+        <v>68.86</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>388.95</v>
+        <v>389.23</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>36</v>
@@ -3452,7 +5116,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>424.95</v>
+        <v>425.23</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="3">
@@ -3475,16 +5139,16 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>66.36</v>
+        <v>66.34999999999999</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>68.76000000000001</v>
+        <v>68.75</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>388.65</v>
+        <v>388.61</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>36</v>
@@ -3496,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>424.65</v>
+        <v>424.61</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="3">
@@ -3519,16 +5183,16 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>66.23999999999999</v>
+        <v>66.20999999999999</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>68.64</v>
+        <v>68.61</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>387.93</v>
+        <v>387.78</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>36</v>
@@ -3540,7 +5204,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>423.93</v>
+        <v>423.78</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="3">
@@ -3563,16 +5227,16 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>66.53</v>
+        <v>66.48</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>68.93000000000001</v>
+        <v>68.88000000000001</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>389.65</v>
+        <v>389.36</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>36</v>
@@ -3584,7 +5248,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>425.65</v>
+        <v>425.36</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="3">
@@ -3658,7 +5322,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="13.75" customWidth="1" style="2" min="2" max="2"/>
   </cols>

</xml_diff>

<commit_message>
more delay matching, update drc rules for better clearance
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -92,15 +92,6 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -467,7 +458,7 @@
       <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.2890625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="29.18" customWidth="1" style="2" min="1" max="1"/>
     <col width="19.72" customWidth="1" style="2" min="2" max="2"/>
@@ -2088,10 +2079,10 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.2890625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="29.18" customWidth="1" style="2" min="1" max="1"/>
     <col width="19.72" customWidth="1" style="2" min="2" max="2"/>
@@ -2370,16 +2361,16 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>22.8</v>
+        <v>22.4</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>23.2</v>
+        <v>22.8</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>158.55</v>
+        <v>155.74</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>4.6</v>
@@ -2391,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>214.45</v>
+        <v>211.64</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
@@ -2414,16 +2405,16 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>20.1</v>
+        <v>19.68</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>20.5</v>
+        <v>20.08</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>139.91</v>
+        <v>136.92</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>4.6</v>
@@ -2435,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>204.71</v>
+        <v>201.72</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">
@@ -2458,16 +2449,16 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>18.27</v>
+        <v>18.06</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>18.67</v>
+        <v>18.46</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>127.35</v>
+        <v>125.82</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>4.6</v>
@@ -2479,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>185.05</v>
+        <v>183.52</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
@@ -2502,16 +2493,16 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>19.71</v>
+        <v>19.39</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>20.11</v>
+        <v>19.79</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>135.84</v>
+        <v>133.61</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>4.6</v>
@@ -2523,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>184.64</v>
+        <v>182.41</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
@@ -2590,16 +2581,16 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>16.21</v>
+        <v>16.02</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>16.61</v>
+        <v>16.42</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>110.75</v>
+        <v>109.4</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>4.6</v>
@@ -2611,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>173.45</v>
+        <v>172.1</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="3">
@@ -2722,16 +2713,16 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>16.06</v>
+        <v>15.9</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>16.46</v>
+        <v>16.3</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>111.69</v>
+        <v>110.52</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>4.6</v>
@@ -2743,7 +2734,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>166.29</v>
+        <v>165.12</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
@@ -3751,7 +3742,7 @@
       <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.42578125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.43359375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="13.06" customWidth="1" style="2" min="2" max="2"/>
     <col width="13.06" customWidth="1" style="2" min="10" max="10"/>
@@ -4335,7 +4326,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.09375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="14.03" customWidth="1" style="2" min="2" max="2"/>
   </cols>
@@ -4962,7 +4953,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.25390625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="3">
       <c r="A1" s="2" t="inlineStr">
@@ -5322,7 +5313,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2890625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="13.75" customWidth="1" style="2" min="2" max="2"/>
   </cols>

</xml_diff>

<commit_message>
length matched DDR_A addr, cmd, ctrl, and byte 0
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DDR_A" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DDR_B" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="eMMC" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RGMII" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ENET" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SD" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QSPI" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
@@ -92,6 +92,15 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -454,8 +463,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -544,12 +553,12 @@
     <row r="2" ht="13.5" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Clock</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D07_A</t>
+          <t>DRAM_CK_A_N</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -557,43 +566,43 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>20.99</v>
+        <v>19.04</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>21.39</v>
+        <v>21.44</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>144.85</v>
+        <v>111.54</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>51.4</v>
+        <v>41.2</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>0</v>
+        <v>-3.35</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>200.85</v>
+        <v>185.39</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Clock</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D05_A</t>
+          <t>DRAM_CK_A_P</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -601,43 +610,43 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>19.98</v>
+        <v>19.02</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>20.38</v>
+        <v>21.42</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>138.13</v>
+        <v>111.29</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>58.1</v>
+        <v>41.1</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0</v>
+        <v>-3.35</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>200.83</v>
+        <v>185.04</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 1 – DQS</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D01_A</t>
+          <t>DRAM_DQS1_A_P</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -645,43 +654,43 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>22.34</v>
+        <v>11.37</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>22.74</v>
+        <v>13.77</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>153.17</v>
+        <v>66.59</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>43</v>
+        <v>48.6</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>200.77</v>
+        <v>151.19</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 1 – DQS</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D06_A</t>
+          <t>DRAM_DQS1_A_N</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -689,439 +698,439 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>18.85</v>
+        <v>11.15</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>19.25</v>
+        <v>13.55</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>131.54</v>
+        <v>65.31999999999999</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>64.59999999999999</v>
+        <v>47.2</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>200.74</v>
+        <v>148.52</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D00_A</t>
+          <t>DRAM_D13_A</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>22.13</v>
+        <v>16.34</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>22.53</v>
+        <v>16.34</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>153.41</v>
+        <v>95.55</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>42.7</v>
+        <v>48.8</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>200.71</v>
+        <v>144.35</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D03_A</t>
+          <t>DRAM_D15_A</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>20.84</v>
+        <v>15.65</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>21.24</v>
+        <v>15.65</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>144.33</v>
+        <v>91.43000000000001</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>51.7</v>
+        <v>52.4</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>200.63</v>
+        <v>143.83</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D04_A</t>
+          <t>DRAM_D14_A</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>19.62</v>
+        <v>13.61</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>20.02</v>
+        <v>13.61</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>136.13</v>
+        <v>79.52</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>59.9</v>
+        <v>58.4</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>200.63</v>
+        <v>137.92</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DMI0_A</t>
+          <t>DRAM_DMI1_A</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>20.16</v>
+        <v>11.47</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>20.56</v>
+        <v>11.47</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>138.62</v>
+        <v>67.05</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>57.2</v>
+        <v>58.6</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>200.42</v>
+        <v>125.65</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D02_A</t>
+          <t>DRAM_D08_A</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>20.36</v>
+        <v>11.87</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>20.76</v>
+        <v>11.87</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>141.08</v>
+        <v>69.28</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>54.6</v>
+        <v>45</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>200.28</v>
+        <v>114.28</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="3">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0 – DQS</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS0_A_P</t>
+          <t>DRAM_D10_A</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, B.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>17.8</v>
+        <v>10.2</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>20.2</v>
+        <v>10.2</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>104.27</v>
+        <v>59.56</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>59</v>
+        <v>46.2</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>199.27</v>
+        <v>105.76</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="3">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 0 – DQS</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS0_A_N</t>
+          <t>DRAM_D09_A</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, B.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>17.8</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>20.2</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>104.16</v>
+        <v>51.74</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>58.9</v>
+        <v>50.1</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>199.06</v>
+        <v>101.84</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="3">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA3_A</t>
+          <t>DRAM_D11_A</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>18.18</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>18.58</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>127.51</v>
+        <v>50.35</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>59.7</v>
+        <v>47.2</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>191.81</v>
+        <v>97.55000000000001</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="3">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 1</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA0_A</t>
+          <t>DRAM_D12_A</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>21.03</v>
+        <v>8.93</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>21.43</v>
+        <v>8.93</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>147.57</v>
+        <v>51.98</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>39.6</v>
+        <v>40.3</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>191.77</v>
+        <v>92.28</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0 – DQS</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CKE0_A</t>
+          <t>DRAM_DQS0_A_P</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1129,43 +1138,43 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu, B.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>19.86</v>
+        <v>17.61</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>1.4</v>
+        <v>2.4</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>21.26</v>
+        <v>20.01</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>138.74</v>
+        <v>103.11</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>20.3</v>
+        <v>36</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>51.2</v>
+        <v>59</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>-18.48</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>191.76</v>
+        <v>198.11</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0 – DQS</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA2_A</t>
+          <t>DRAM_DQS0_A_N</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1173,43 +1182,43 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>18.87</v>
+        <v>17.61</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0.4</v>
+        <v>2.4</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>19.27</v>
+        <v>20.01</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>132.31</v>
+        <v>102.99</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>4.6</v>
+        <v>36</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>54.8</v>
+        <v>58.9</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>191.71</v>
+        <v>197.89</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" s="3">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA5_A</t>
+          <t>DRAM_D07_A</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1221,39 +1230,39 @@
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>22.08</v>
+        <v>20.84</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>22.48</v>
+        <v>21.24</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>155.11</v>
+        <v>142</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>32</v>
+        <v>51.4</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>191.71</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" s="3">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CKE1_A</t>
+          <t>DRAM_D03_A</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1261,43 +1270,43 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu, B.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>21.45</v>
+        <v>20.52</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>22.85</v>
+        <v>20.92</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>149.96</v>
+        <v>141.7</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>20.3</v>
+        <v>4.6</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>39.9</v>
+        <v>51.7</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>-18.48</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>191.68</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" s="3">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>~{DRAM_CS1_A}</t>
+          <t>DRAM_DMI0_A</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1309,39 +1318,39 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>20.35</v>
+        <v>19.82</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>20.75</v>
+        <v>20.22</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>142.76</v>
+        <v>136.17</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>44.2</v>
+        <v>57.2</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>191.56</v>
+        <v>197.97</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA1_A</t>
+          <t>DRAM_D05_A</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1353,39 +1362,39 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>22.47</v>
+        <v>19.57</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>22.87</v>
+        <v>19.97</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>157.8</v>
+        <v>135.21</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>29.1</v>
+        <v>58.1</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>191.5</v>
+        <v>197.91</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" s="3">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA4_A</t>
+          <t>DRAM_D01_A</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1397,39 +1406,39 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>21.8</v>
+        <v>22.79</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>22.2</v>
+        <v>23.19</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>153.03</v>
+        <v>150.29</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>33.8</v>
+        <v>43</v>
       </c>
       <c r="K21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>191.43</v>
+        <v>197.89</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Address, Command and Control</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>~{DRAM_CS0_A}</t>
+          <t>DRAM_D06_A</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1441,39 +1450,39 @@
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>21.49</v>
+        <v>18.88</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>21.89</v>
+        <v>19.28</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>150.82</v>
+        <v>128.6</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>35.9</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="K22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>191.32</v>
+        <v>197.8</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>Clock</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CK_A_N</t>
+          <t>DRAM_D00_A</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1481,43 +1490,43 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, B.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>19.7</v>
+        <v>21.89</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>22.1</v>
+        <v>22.29</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>115.37</v>
+        <v>150.43</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>36</v>
+        <v>4.6</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>41.2</v>
+        <v>42.7</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>-3.35</v>
+        <v>0</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>189.22</v>
+        <v>197.73</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Clock</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CK_A_P</t>
+          <t>DRAM_D02_A</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1525,219 +1534,219 @@
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, B.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>19.68</v>
+        <v>20.04</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>22.08</v>
+        <v>20.44</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>115.12</v>
+        <v>138.45</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>36</v>
+        <v>4.6</v>
       </c>
       <c r="J24" s="2" t="n">
-        <v>41.1</v>
+        <v>54.6</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>-3.35</v>
+        <v>0</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>188.87</v>
+        <v>197.65</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" s="3">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Byte Lane 0</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D13_A</t>
+          <t>DRAM_D04_A</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>16.38</v>
+        <v>19.23</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>16.38</v>
+        <v>19.63</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>95.88</v>
+        <v>133.31</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J25" s="2" t="n">
-        <v>48.8</v>
+        <v>59.9</v>
       </c>
       <c r="K25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>144.68</v>
+        <v>197.81</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" s="3">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D12_A</t>
+          <t>DRAM_CA3_A</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>17.86</v>
+        <v>18.49</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>17.86</v>
+        <v>18.89</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>104.35</v>
+        <v>129.63</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J26" s="2" t="n">
-        <v>40.3</v>
+        <v>59.7</v>
       </c>
       <c r="K26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L26" s="2" t="n">
-        <v>144.65</v>
+        <v>193.93</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1" s="3">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D08_A</t>
+          <t>~{DRAM_CS0_A}</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>17.06</v>
+        <v>21.85</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>17.06</v>
+        <v>22.25</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>99.59999999999999</v>
+        <v>153.42</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>45</v>
+        <v>35.9</v>
       </c>
       <c r="K27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>144.6</v>
+        <v>193.92</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1" s="3">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D11_A</t>
+          <t>DRAM_CA0_A</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>16.66</v>
+        <v>21.33</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>16.66</v>
+        <v>21.73</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>97.29000000000001</v>
+        <v>149.71</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J28" s="2" t="n">
-        <v>47.2</v>
+        <v>39.6</v>
       </c>
       <c r="K28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L28" s="2" t="n">
-        <v>144.49</v>
+        <v>193.91</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1" s="3">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1 – DQS</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS1_A_P</t>
+          <t>DRAM_CKE0_A</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -1745,87 +1754,87 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, B.Cu</t>
+          <t>F.Cu, In2.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>10.22</v>
+        <v>20.14</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>2.4</v>
+        <v>1.4</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>12.62</v>
+        <v>21.54</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>59.84</v>
+        <v>140.87</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>36</v>
+        <v>20.3</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>48.6</v>
+        <v>51.2</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0</v>
+        <v>-18.48</v>
       </c>
       <c r="L29" s="2" t="n">
-        <v>144.44</v>
+        <v>193.89</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1" s="3">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D09_A</t>
+          <t>DRAM_CA5_A</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>16.15</v>
+        <v>22.39</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>16.15</v>
+        <v>22.79</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>94.31999999999999</v>
+        <v>157.28</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J30" s="2" t="n">
-        <v>50.1</v>
+        <v>32</v>
       </c>
       <c r="K30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L30" s="2" t="n">
-        <v>144.42</v>
+        <v>193.88</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="3">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1 – DQS</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS1_A_N</t>
+          <t>DRAM_CKE1_A</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -1833,208 +1842,208 @@
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, B.Cu</t>
+          <t>F.Cu, In2.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>10.44</v>
+        <v>21.73</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>2.4</v>
+        <v>1.4</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>12.84</v>
+        <v>23.13</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>61.17</v>
+        <v>152.14</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>36</v>
+        <v>20.3</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>47.2</v>
+        <v>39.9</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>0</v>
+        <v>-18.48</v>
       </c>
       <c r="L31" s="2" t="n">
-        <v>144.37</v>
+        <v>193.86</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1" s="3">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DMI1_A</t>
+          <t>DRAM_CA1_A</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>14.68</v>
+        <v>22.81</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>14.68</v>
+        <v>23.21</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>85.77</v>
+        <v>160.16</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J32" s="2" t="n">
-        <v>58.6</v>
+        <v>29.1</v>
       </c>
       <c r="K32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>144.37</v>
+        <v>193.86</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1" s="3">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D10_A</t>
+          <t>~{DRAM_CS1_A}</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>16.77</v>
+        <v>20.66</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>16.77</v>
+        <v>21.06</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>98.01000000000001</v>
+        <v>145.01</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J33" s="2" t="n">
-        <v>46.2</v>
+        <v>44.2</v>
       </c>
       <c r="K33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L33" s="2" t="n">
-        <v>144.21</v>
+        <v>193.81</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1" s="3">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D14_A</t>
+          <t>DRAM_CA2_A</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>14.68</v>
+        <v>19.16</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>14.68</v>
+        <v>19.56</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>85.73999999999999</v>
+        <v>134.39</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J34" s="2" t="n">
-        <v>58.4</v>
+        <v>54.8</v>
       </c>
       <c r="K34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L34" s="2" t="n">
-        <v>144.14</v>
+        <v>193.79</v>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1" s="3">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>Byte Lane 1</t>
+          <t>Address, Command and Control</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D15_A</t>
+          <t>DRAM_CA4_A</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" s="2" t="inlineStr">
         <is>
-          <t>F.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>15.67</v>
+        <v>22.13</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>15.67</v>
+        <v>22.53</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>91.64</v>
+        <v>155.38</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="J35" s="2" t="n">
-        <v>52.4</v>
+        <v>33.8</v>
       </c>
       <c r="K35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L35" s="2" t="n">
-        <v>144.04</v>
+        <v>193.78</v>
       </c>
     </row>
     <row r="36" ht="13.5" customHeight="1" s="3"/>
@@ -2078,7 +2087,7 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
@@ -2361,16 +2370,16 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>22.4</v>
+        <v>22.17</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>22.8</v>
+        <v>22.57</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>155.74</v>
+        <v>154.1</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>4.6</v>
@@ -2382,7 +2391,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>211.64</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
@@ -2405,16 +2414,16 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>19.68</v>
+        <v>19.47</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>20.08</v>
+        <v>19.87</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>136.92</v>
+        <v>135.46</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>4.6</v>
@@ -2426,7 +2435,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>201.72</v>
+        <v>200.26</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">
@@ -2449,16 +2458,16 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>18.06</v>
+        <v>17.8</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>18.46</v>
+        <v>18.2</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>125.82</v>
+        <v>124.01</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>4.6</v>
@@ -2470,7 +2479,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>183.52</v>
+        <v>181.71</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
@@ -2493,16 +2502,16 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>19.39</v>
+        <v>19.16</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>19.79</v>
+        <v>19.56</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>133.61</v>
+        <v>131.97</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>4.6</v>
@@ -2514,7 +2523,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>182.41</v>
+        <v>180.77</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
@@ -2537,16 +2546,16 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>16.87</v>
+        <v>17.17</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>17.27</v>
+        <v>17.57</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>115.84</v>
+        <v>117.7</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>4.6</v>
@@ -2558,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>178.44</v>
+        <v>180.3</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="3">
@@ -2581,16 +2590,16 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>16.02</v>
+        <v>15.72</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>16.42</v>
+        <v>16.12</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>109.4</v>
+        <v>106.3</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>4.6</v>
@@ -2602,7 +2611,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>172.1</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="3">
@@ -2625,16 +2634,16 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>17.16</v>
+        <v>17.85</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>17.56</v>
+        <v>18.25</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>116.78</v>
+        <v>120.21</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>4.6</v>
@@ -2646,7 +2655,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>170.18</v>
+        <v>173.61</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="3">
@@ -2669,16 +2678,16 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>15.23</v>
+        <v>15.14</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>15.63</v>
+        <v>15.54</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>103.8</v>
+        <v>103.22</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>4.6</v>
@@ -2690,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>167.5</v>
+        <v>166.92</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="3">
@@ -2713,16 +2722,16 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>15.9</v>
+        <v>16.09</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>16.3</v>
+        <v>16.49</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>110.52</v>
+        <v>111.88</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>4.6</v>
@@ -2734,7 +2743,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>165.12</v>
+        <v>166.48</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
@@ -2757,16 +2766,16 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>11</v>
+        <v>10.79</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>13.4</v>
+        <v>13.19</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>64.41</v>
+        <v>63.18</v>
       </c>
       <c r="I15" s="2" t="n">
         <v>36</v>
@@ -2778,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>149.01</v>
+        <v>147.78</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
@@ -2801,16 +2810,16 @@
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>11</v>
+        <v>10.59</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>13.4</v>
+        <v>12.99</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>64.41</v>
+        <v>62.05</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>36</v>
@@ -2822,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>149.01</v>
+        <v>146.65</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" s="3">
@@ -2854,7 +2863,7 @@
         <v>13.37</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>78.12</v>
+        <v>78.05</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>0</v>
@@ -2866,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>126.12</v>
+        <v>126.05</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" s="3">
@@ -2933,16 +2942,16 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>11.19</v>
+        <v>10.95</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>11.19</v>
+        <v>10.95</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>65.34</v>
+        <v>63.86</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>0</v>
@@ -2954,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>118.94</v>
+        <v>117.46</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
@@ -2986,7 +2995,7 @@
         <v>10.8</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>63.15</v>
+        <v>63.12</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>0</v>
@@ -2998,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>117.85</v>
+        <v>117.82</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" s="3">
@@ -3030,7 +3039,7 @@
         <v>9.289999999999999</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>54.25</v>
+        <v>54.26</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>0</v>
@@ -3042,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>107.05</v>
+        <v>107.06</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
@@ -3074,7 +3083,7 @@
         <v>9.42</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>54.95</v>
+        <v>54.93</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
@@ -3086,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>106.45</v>
+        <v>106.43</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
@@ -3109,16 +3118,16 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>8.67</v>
+        <v>8.5</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>8.67</v>
+        <v>8.5</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>50.8</v>
+        <v>49.64</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>0</v>
@@ -3130,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>105.3</v>
+        <v>104.14</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">
@@ -3162,7 +3171,7 @@
         <v>8.48</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>49.41</v>
+        <v>49.44</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>0</v>
@@ -3174,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>99.31</v>
+        <v>99.34</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" s="3">
@@ -3197,16 +3206,16 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>9.289999999999999</v>
+        <v>8.57</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>9.289999999999999</v>
+        <v>8.57</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>54.24</v>
+        <v>49.87</v>
       </c>
       <c r="I25" s="2" t="n">
         <v>0</v>
@@ -3218,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>96.24000000000001</v>
+        <v>91.87</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" s="3">
@@ -3241,16 +3250,16 @@
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>19.66</v>
+        <v>16.33</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>1.4</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>21.06</v>
+        <v>17.73</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>137.32</v>
+        <v>113.72</v>
       </c>
       <c r="I26" s="2" t="n">
         <v>20.3</v>
@@ -3262,7 +3271,7 @@
         <v>-18.48</v>
       </c>
       <c r="L26" s="2" t="n">
-        <v>190.74</v>
+        <v>167.14</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1" s="3">
@@ -3285,16 +3294,16 @@
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>21.6</v>
+        <v>10.65</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>22</v>
+        <v>11.05</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>151.65</v>
+        <v>74.11</v>
       </c>
       <c r="I27" s="2" t="n">
         <v>4.6</v>
@@ -3306,7 +3315,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>190.65</v>
+        <v>113.11</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1" s="3">
@@ -3329,16 +3338,16 @@
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>19.64</v>
+        <v>13.29</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>1.4</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>21.04</v>
+        <v>14.69</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>137.16</v>
+        <v>92.25</v>
       </c>
       <c r="I28" s="2" t="n">
         <v>20.3</v>
@@ -3350,7 +3359,7 @@
         <v>-18.48</v>
       </c>
       <c r="L28" s="2" t="n">
-        <v>190.58</v>
+        <v>145.67</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1" s="3">
@@ -3373,16 +3382,16 @@
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>21.11</v>
+        <v>21.19</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>21.51</v>
+        <v>21.59</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>147.56</v>
+        <v>148.14</v>
       </c>
       <c r="I29" s="2" t="n">
         <v>4.6</v>
@@ -3394,7 +3403,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="2" t="n">
-        <v>190.76</v>
+        <v>191.34</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1" s="3">
@@ -3417,16 +3426,16 @@
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>21.65</v>
+        <v>19.15</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>22.05</v>
+        <v>19.55</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>151.97</v>
+        <v>134.28</v>
       </c>
       <c r="I30" s="2" t="n">
         <v>4.6</v>
@@ -3438,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="2" t="n">
-        <v>190.87</v>
+        <v>173.18</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="3">
@@ -3461,16 +3470,16 @@
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>21.98</v>
+        <v>10.72</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>22.38</v>
+        <v>11.12</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>154.34</v>
+        <v>74.62</v>
       </c>
       <c r="I31" s="2" t="n">
         <v>4.6</v>
@@ -3482,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="2" t="n">
-        <v>190.84</v>
+        <v>111.12</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1" s="3">
@@ -3505,16 +3514,16 @@
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>18.52</v>
+        <v>18.04</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>18.92</v>
+        <v>18.44</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>129.82</v>
+        <v>126.43</v>
       </c>
       <c r="I32" s="2" t="n">
         <v>4.6</v>
@@ -3526,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>190.92</v>
+        <v>187.53</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1" s="3">
@@ -3549,16 +3558,16 @@
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>20.84</v>
+        <v>13.54</v>
       </c>
       <c r="F33" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>21.24</v>
+        <v>13.94</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>146.22</v>
+        <v>94.56999999999999</v>
       </c>
       <c r="I33" s="2" t="n">
         <v>4.6</v>
@@ -3570,7 +3579,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="2" t="n">
-        <v>190.82</v>
+        <v>139.17</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1" s="3">
@@ -3593,16 +3602,16 @@
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>19.76</v>
+        <v>10.63</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>20.16</v>
+        <v>11.03</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>138.57</v>
+        <v>73.95</v>
       </c>
       <c r="I34" s="2" t="n">
         <v>4.6</v>
@@ -3614,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="2" t="n">
-        <v>190.87</v>
+        <v>126.25</v>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1" s="3">
@@ -3637,16 +3646,16 @@
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>18.1</v>
+        <v>17.89</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>18.5</v>
+        <v>18.29</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>126.82</v>
+        <v>125.36</v>
       </c>
       <c r="I35" s="2" t="n">
         <v>4.6</v>
@@ -3658,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="2" t="n">
-        <v>190.92</v>
+        <v>189.46</v>
       </c>
     </row>
     <row r="36" ht="13.5" customHeight="1" s="3">
@@ -3835,16 +3844,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>27.46</v>
+        <v>27.49</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>27.46</v>
+        <v>27.49</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>160.6</v>
+        <v>160.8</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>0</v>
@@ -3856,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>160.6</v>
+        <v>160.8</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="3">
@@ -3879,16 +3888,16 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>23.88</v>
+        <v>23.96</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>23.88</v>
+        <v>23.96</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>139.4</v>
+        <v>139.87</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>0</v>
@@ -3900,7 +3909,7 @@
         <v>20.9</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>160.3</v>
+        <v>160.77</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="3">
@@ -3923,16 +3932,16 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>27.39</v>
+        <v>26.32</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>27.39</v>
+        <v>26.32</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>160.19</v>
+        <v>153.89</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>0</v>
@@ -3944,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>160.19</v>
+        <v>153.89</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="3">
@@ -3967,16 +3976,16 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>27.32</v>
+        <v>27.4</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>27.32</v>
+        <v>27.4</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>159.9</v>
+        <v>160.37</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>0</v>
@@ -3988,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>159.9</v>
+        <v>160.37</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="3">
@@ -4011,16 +4020,16 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>27.2</v>
+        <v>27.28</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>27.2</v>
+        <v>27.28</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>159.21</v>
+        <v>159.68</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>0</v>
@@ -4032,7 +4041,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>159.21</v>
+        <v>159.68</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="3">
@@ -4055,16 +4064,16 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>27.2</v>
+        <v>27.28</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>27.2</v>
+        <v>27.28</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>159.18</v>
+        <v>159.65</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>0</v>
@@ -4076,7 +4085,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>159.18</v>
+        <v>159.65</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="3">
@@ -4099,16 +4108,16 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>27.1</v>
+        <v>27.18</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>27.1</v>
+        <v>27.18</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>158.58</v>
+        <v>159.04</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>0</v>
@@ -4120,7 +4129,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>158.58</v>
+        <v>159.04</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="3">
@@ -4143,16 +4152,16 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>26.97</v>
+        <v>27.05</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>26.97</v>
+        <v>27.05</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>157.83</v>
+        <v>158.3</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>0</v>
@@ -4164,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>157.83</v>
+        <v>158.3</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="3">
@@ -4187,16 +4196,16 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>26.95</v>
+        <v>27.03</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>26.95</v>
+        <v>27.03</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>157.74</v>
+        <v>158.21</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>0</v>
@@ -4208,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>157.74</v>
+        <v>158.21</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="3">
@@ -4231,16 +4240,16 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>26.94</v>
+        <v>26.97</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>26.94</v>
+        <v>26.97</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>157.42</v>
+        <v>157.61</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>0</v>
@@ -4252,7 +4261,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>157.42</v>
+        <v>157.61</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="3">
@@ -4275,16 +4284,16 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>26.87</v>
+        <v>26.95</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>26.87</v>
+        <v>26.95</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>157.26</v>
+        <v>157.73</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>0</v>
@@ -4296,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>157.26</v>
+        <v>157.73</v>
       </c>
     </row>
   </sheetData>
@@ -4320,10 +4329,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -4770,16 +4779,16 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>12.93</v>
+        <v>13.23</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>13.33</v>
+        <v>13.63</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>81.77</v>
+        <v>83.94</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>4.6</v>
@@ -4791,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>86.36999999999999</v>
+        <v>88.53999999999999</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="3">
@@ -4924,6 +4933,358 @@
       </c>
       <c r="L13" s="2" t="n">
         <v>79.05999999999999</v>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1" s="3">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI0</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>TRD0_P</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>21.22</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>21.22</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>121.66</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>121.66</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1" s="3">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI0</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>TRD0_N</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>21.22</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>21.22</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>121.66</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>121.66</v>
+      </c>
+    </row>
+    <row r="16" ht="12.75" customHeight="1" s="3">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI1</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>TRD1_P</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>22.65</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>25.05</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>129.87</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>165.87</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" customHeight="1" s="3">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI1</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>TRD1_N</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>22.65</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>25.05</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>129.87</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>165.87</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1" s="3">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI2</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>TRD2_P</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>22.55</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>24.95</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>129.29</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>165.29</v>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1" s="3">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI2</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>TRD2_N</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>22.55</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>24.95</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>129.28</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>165.28</v>
+      </c>
+    </row>
+    <row r="20" ht="12.75" customHeight="1" s="3">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI3</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>TRD3_P</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>25.44</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>132.12</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>168.12</v>
+      </c>
+    </row>
+    <row r="21" ht="12.75" customHeight="1" s="3">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MDI3</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>TRD3_N</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>F.Cu, B.Cu</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>25.44</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>132.12</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>168.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
length matched DDR_A byte 1
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -92,15 +92,6 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -464,7 +455,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="A36:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -658,16 +649,16 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11.37</v>
+        <v>11.44</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>13.77</v>
+        <v>13.84</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>66.59</v>
+        <v>67.03</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>36</v>
@@ -679,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>151.19</v>
+        <v>151.63</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
@@ -702,16 +693,16 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>11.15</v>
+        <v>11.71</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>13.55</v>
+        <v>14.11</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>65.31999999999999</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>36</v>
@@ -723,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>148.52</v>
+        <v>151.8</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
@@ -746,16 +737,16 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>16.34</v>
+        <v>17.58</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>16.34</v>
+        <v>17.58</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>95.55</v>
+        <v>102.83</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>0</v>
@@ -767,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>144.35</v>
+        <v>151.63</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
@@ -790,16 +781,16 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>15.65</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>15.65</v>
+        <v>17</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>91.43000000000001</v>
+        <v>99.31</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>0</v>
@@ -811,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>143.83</v>
+        <v>151.71</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">
@@ -834,16 +825,16 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>13.61</v>
+        <v>15.97</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>13.61</v>
+        <v>15.97</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>79.52</v>
+        <v>93.39</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>0</v>
@@ -855,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>137.92</v>
+        <v>151.79</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
@@ -878,16 +869,16 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>11.47</v>
+        <v>15.9</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>11.47</v>
+        <v>15.9</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>67.05</v>
+        <v>92.97</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>0</v>
@@ -899,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>125.65</v>
+        <v>151.57</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
@@ -922,16 +913,16 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>11.87</v>
+        <v>18.25</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>11.87</v>
+        <v>18.25</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>69.28</v>
+        <v>106.62</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>0</v>
@@ -943,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>114.28</v>
+        <v>151.62</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="3">
@@ -966,16 +957,16 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>10.2</v>
+        <v>18.03</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>10.2</v>
+        <v>18.03</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>59.56</v>
+        <v>105.4</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>0</v>
@@ -987,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>105.76</v>
+        <v>151.6</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="3">
@@ -1010,16 +1001,16 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>8.880000000000001</v>
+        <v>17.36</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>8.880000000000001</v>
+        <v>17.36</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>51.74</v>
+        <v>101.44</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>0</v>
@@ -1031,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>101.84</v>
+        <v>151.54</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="3">
@@ -1054,16 +1045,16 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>8.640000000000001</v>
+        <v>17.86</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>8.640000000000001</v>
+        <v>17.86</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>50.35</v>
+        <v>104.38</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>0</v>
@@ -1075,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>97.55000000000001</v>
+        <v>151.58</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="3">
@@ -1098,16 +1089,16 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>8.93</v>
+        <v>19.06</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>8.93</v>
+        <v>19.06</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>51.98</v>
+        <v>111.3</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>0</v>
@@ -1119,7 +1110,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>92.28</v>
+        <v>151.6</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
@@ -2088,7 +2079,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
+      <selection pane="topLeft" activeCell="I39" activeCellId="1" sqref="A36:B36 I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -3748,7 +3739,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+      <selection pane="topLeft" activeCell="L12" activeCellId="1" sqref="A36:B36 L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.43359375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -4332,7 +4323,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="A36:B36 B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -5311,7 +5302,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A36:B36 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -5671,7 +5662,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A36:B36 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.2890625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>

<commit_message>
length matched DDR_B byte 1
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DDR_A" sheetId="1" state="visible" r:id="rId1"/>
@@ -92,6 +92,15 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -454,8 +463,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="A36:B36"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -637,7 +646,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS1_A_P</t>
+          <t>DRAM_DQS1_A_N</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -649,28 +658,28 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>11.44</v>
+        <v>11.71</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>13.84</v>
+        <v>14.11</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>67.03</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>36</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>48.6</v>
+        <v>47.2</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>151.63</v>
+        <v>151.8</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
@@ -681,7 +690,7 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS1_A_N</t>
+          <t>DRAM_DQS1_A_P</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -693,28 +702,28 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>11.71</v>
+        <v>11.44</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>14.11</v>
+        <v>13.84</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>68.59999999999999</v>
+        <v>67.03</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>36</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>47.2</v>
+        <v>48.6</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>151.8</v>
+        <v>151.63</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
@@ -725,7 +734,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D13_A</t>
+          <t>DRAM_D14_A</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -737,28 +746,28 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>17.58</v>
+        <v>15.97</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>17.58</v>
+        <v>15.97</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>102.83</v>
+        <v>93.39</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>48.8</v>
+        <v>58.4</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>151.63</v>
+        <v>151.79</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
@@ -813,7 +822,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D14_A</t>
+          <t>DRAM_D13_A</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -825,28 +834,28 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>15.97</v>
+        <v>17.58</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>15.97</v>
+        <v>17.58</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>93.39</v>
+        <v>102.83</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>58.4</v>
+        <v>48.8</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>151.79</v>
+        <v>151.63</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
@@ -857,7 +866,7 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DMI1_A</t>
+          <t>DRAM_D08_A</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -869,28 +878,28 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>15.9</v>
+        <v>18.25</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>15.9</v>
+        <v>18.25</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>92.97</v>
+        <v>106.62</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>58.6</v>
+        <v>45</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>151.57</v>
+        <v>151.62</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
@@ -901,7 +910,7 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D08_A</t>
+          <t>DRAM_D10_A</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -913,28 +922,28 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>18.25</v>
+        <v>18.03</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>18.25</v>
+        <v>18.03</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>106.62</v>
+        <v>105.4</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>45</v>
+        <v>46.2</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>151.62</v>
+        <v>151.6</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="3">
@@ -945,7 +954,7 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D10_A</t>
+          <t>DRAM_D12_A</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -957,22 +966,22 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>18.03</v>
+        <v>19.06</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>18.03</v>
+        <v>19.06</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>105.4</v>
+        <v>111.3</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>46.2</v>
+        <v>40.3</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>0</v>
@@ -989,7 +998,7 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D09_A</t>
+          <t>DRAM_D11_A</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1001,28 +1010,28 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>17.36</v>
+        <v>17.86</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>17.36</v>
+        <v>17.86</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>101.44</v>
+        <v>104.38</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>50.1</v>
+        <v>47.2</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>151.54</v>
+        <v>151.58</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="3">
@@ -1033,7 +1042,7 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D11_A</t>
+          <t>DRAM_DMI1_A</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1045,28 +1054,28 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>17.86</v>
+        <v>15.9</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>17.86</v>
+        <v>15.9</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>104.38</v>
+        <v>92.97</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>47.2</v>
+        <v>58.6</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>151.58</v>
+        <v>151.57</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="3">
@@ -1077,7 +1086,7 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D12_A</t>
+          <t>DRAM_D09_A</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1089,28 +1098,28 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>19.06</v>
+        <v>17.36</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>19.06</v>
+        <v>17.36</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>111.3</v>
+        <v>101.44</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>40.3</v>
+        <v>50.1</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>151.6</v>
+        <v>151.54</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
@@ -1429,7 +1438,7 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D06_A</t>
+          <t>DRAM_D04_A</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1441,28 +1450,28 @@
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>18.88</v>
+        <v>19.23</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>19.28</v>
+        <v>19.63</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>128.6</v>
+        <v>133.31</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>64.59999999999999</v>
+        <v>59.9</v>
       </c>
       <c r="K22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>197.8</v>
+        <v>197.81</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
@@ -1473,7 +1482,7 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D00_A</t>
+          <t>DRAM_D06_A</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1485,28 +1494,28 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>21.89</v>
+        <v>18.88</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>22.29</v>
+        <v>19.28</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>150.43</v>
+        <v>128.6</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>42.7</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="K23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>197.73</v>
+        <v>197.8</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">
@@ -1517,7 +1526,7 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D02_A</t>
+          <t>DRAM_D00_A</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1529,28 +1538,28 @@
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>20.04</v>
+        <v>21.89</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>20.44</v>
+        <v>22.29</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>138.45</v>
+        <v>150.43</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J24" s="2" t="n">
-        <v>54.6</v>
+        <v>42.7</v>
       </c>
       <c r="K24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>197.65</v>
+        <v>197.73</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" s="3">
@@ -1561,7 +1570,7 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D04_A</t>
+          <t>DRAM_D02_A</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -1573,28 +1582,28 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>19.23</v>
+        <v>20.04</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>19.63</v>
+        <v>20.44</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>133.31</v>
+        <v>138.45</v>
       </c>
       <c r="I25" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J25" s="2" t="n">
-        <v>59.9</v>
+        <v>54.6</v>
       </c>
       <c r="K25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>197.81</v>
+        <v>197.65</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" s="3">
@@ -2078,8 +2087,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I39" activeCellId="1" sqref="A36:B36 I39"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J42" activeCellId="0" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -2317,16 +2326,16 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>18.4</v>
+        <v>18.63</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>20.8</v>
+        <v>21.03</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>107.64</v>
+        <v>108.97</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>36</v>
@@ -2338,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>199.14</v>
+        <v>200.47</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
@@ -2349,7 +2358,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D09_B</t>
+          <t>DRAM_D08_B</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -2361,28 +2370,28 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>22.17</v>
+        <v>19.43</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>22.57</v>
+        <v>19.83</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>154.1</v>
+        <v>135.14</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>51.3</v>
+        <v>60.2</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>210</v>
+        <v>199.94</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="3">
@@ -2393,7 +2402,7 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D08_B</t>
+          <t>DRAM_DMI1_B</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -2405,28 +2414,28 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>19.47</v>
+        <v>20.37</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>19.87</v>
+        <v>20.77</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>135.46</v>
+        <v>142.22</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>60.2</v>
+        <v>53.1</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>200.26</v>
+        <v>199.92</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="3">
@@ -2437,7 +2446,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DMI1_B</t>
+          <t>DRAM_D13_B</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -2449,28 +2458,28 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>17.8</v>
+        <v>20.08</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>18.2</v>
+        <v>20.48</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>124.01</v>
+        <v>137.2</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>53.1</v>
+        <v>58.1</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>181.71</v>
+        <v>199.9</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="3">
@@ -2481,7 +2490,7 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D15_B</t>
+          <t>DRAM_D09_B</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -2493,28 +2502,28 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>19.16</v>
+        <v>20.73</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>19.56</v>
+        <v>21.13</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>131.97</v>
+        <v>143.98</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>44.2</v>
+        <v>51.3</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>180.77</v>
+        <v>199.88</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="3">
@@ -2525,7 +2534,7 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D11_B</t>
+          <t>DRAM_D12_B</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -2537,28 +2546,28 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>17.17</v>
+        <v>19.86</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>17.57</v>
+        <v>20.26</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>117.7</v>
+        <v>136.17</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>58</v>
+        <v>59.1</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>180.3</v>
+        <v>199.87</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="3">
@@ -2569,7 +2578,7 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D13_B</t>
+          <t>DRAM_D11_B</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -2581,28 +2590,28 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>15.72</v>
+        <v>19.94</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>16.12</v>
+        <v>20.34</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>106.3</v>
+        <v>137.25</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>58.1</v>
+        <v>58</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>169</v>
+        <v>199.85</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="3">
@@ -2613,7 +2622,7 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D10_B</t>
+          <t>DRAM_D14_B</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -2625,28 +2634,28 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>17.85</v>
+        <v>20.81</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>18.25</v>
+        <v>21.21</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>120.21</v>
+        <v>145.25</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>48.8</v>
+        <v>50</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>173.61</v>
+        <v>199.85</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="3">
@@ -2657,7 +2666,7 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D12_B</t>
+          <t>DRAM_D10_B</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -2669,28 +2678,28 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>15.14</v>
+        <v>21.55</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>15.54</v>
+        <v>21.95</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>103.22</v>
+        <v>146.4</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>59.1</v>
+        <v>48.8</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>166.92</v>
+        <v>199.8</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="3">
@@ -2701,7 +2710,7 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D14_B</t>
+          <t>DRAM_D15_B</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -2713,28 +2722,28 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>16.09</v>
+        <v>21.85</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>16.49</v>
+        <v>22.25</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>111.88</v>
+        <v>150.98</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>50</v>
+        <v>44.2</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>166.48</v>
+        <v>199.78</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
@@ -2921,7 +2930,7 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D04_B</t>
+          <t>DRAM_D06_B</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -2933,28 +2942,28 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>10.95</v>
+        <v>10.8</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>10.95</v>
+        <v>10.8</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>63.86</v>
+        <v>63.12</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>53.6</v>
+        <v>54.7</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>117.46</v>
+        <v>117.82</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
@@ -2965,7 +2974,7 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D06_B</t>
+          <t>DRAM_D04_B</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -2977,28 +2986,28 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>10.8</v>
+        <v>10.95</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>10.8</v>
+        <v>10.95</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>63.12</v>
+        <v>63.86</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>54.7</v>
+        <v>53.6</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>117.82</v>
+        <v>117.46</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" s="3">
@@ -3229,7 +3238,7 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CKE1_B</t>
+          <t>DRAM_CA5_B</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -3237,32 +3246,32 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu, B.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>16.33</v>
+        <v>20.91</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>17.73</v>
+        <v>21.31</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>113.72</v>
+        <v>146.14</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>20.3</v>
+        <v>4.6</v>
       </c>
       <c r="J26" s="2" t="n">
-        <v>51.6</v>
+        <v>38.6</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>-18.48</v>
+        <v>0</v>
       </c>
       <c r="L26" s="2" t="n">
-        <v>167.14</v>
+        <v>189.34</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1" s="3">
@@ -3273,7 +3282,7 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA1_B</t>
+          <t>DRAM_CA2_B</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -3285,28 +3294,28 @@
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>10.65</v>
+        <v>17.87</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>11.05</v>
+        <v>18.27</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>74.11</v>
+        <v>125.21</v>
       </c>
       <c r="I27" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>34.4</v>
+        <v>59.5</v>
       </c>
       <c r="K27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>113.11</v>
+        <v>189.31</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1" s="3">
@@ -3317,7 +3326,7 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CKE0_B</t>
+          <t>DRAM_CA4_B</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -3325,32 +3334,32 @@
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu, B.Cu</t>
+          <t>F.Cu, In2.Cu</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>13.29</v>
+        <v>21.42</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>14.69</v>
+        <v>21.82</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>92.25</v>
+        <v>150.35</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>20.3</v>
+        <v>4.6</v>
       </c>
       <c r="J28" s="2" t="n">
-        <v>51.6</v>
+        <v>34.3</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>-18.48</v>
+        <v>0</v>
       </c>
       <c r="L28" s="2" t="n">
-        <v>145.67</v>
+        <v>189.25</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1" s="3">
@@ -3361,7 +3370,7 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA5_B</t>
+          <t>DRAM_CA1_B</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -3373,28 +3382,28 @@
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>21.19</v>
+        <v>21.41</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>21.59</v>
+        <v>21.81</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>148.14</v>
+        <v>150.25</v>
       </c>
       <c r="I29" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>38.6</v>
+        <v>34.4</v>
       </c>
       <c r="K29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L29" s="2" t="n">
-        <v>191.34</v>
+        <v>189.25</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1" s="3">
@@ -3405,7 +3414,7 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA4_B</t>
+          <t>DRAM_CA0_B</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -3417,28 +3426,28 @@
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>19.15</v>
+        <v>21.76</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>19.55</v>
+        <v>22.16</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>134.28</v>
+        <v>152.72</v>
       </c>
       <c r="I30" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J30" s="2" t="n">
-        <v>34.3</v>
+        <v>31.9</v>
       </c>
       <c r="K30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L30" s="2" t="n">
-        <v>173.18</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="3">
@@ -3449,7 +3458,7 @@
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA0_B</t>
+          <t>DRAM_CKE1_B</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -3457,32 +3466,32 @@
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, In2.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>10.72</v>
+        <v>19.44</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>11.12</v>
+        <v>20.84</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>74.62</v>
+        <v>135.78</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>4.6</v>
+        <v>20.3</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>31.9</v>
+        <v>51.6</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>0</v>
+        <v>-18.48</v>
       </c>
       <c r="L31" s="2" t="n">
-        <v>111.12</v>
+        <v>189.2</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1" s="3">
@@ -3493,7 +3502,7 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA3_B</t>
+          <t>~{DRAM_CS1_B}</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -3505,28 +3514,28 @@
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>18.04</v>
+        <v>19.52</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>18.44</v>
+        <v>19.92</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>126.43</v>
+        <v>136.9</v>
       </c>
       <c r="I32" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J32" s="2" t="n">
-        <v>56.5</v>
+        <v>47.7</v>
       </c>
       <c r="K32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>187.53</v>
+        <v>189.2</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1" s="3">
@@ -3549,16 +3558,16 @@
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>13.54</v>
+        <v>20.6</v>
       </c>
       <c r="F33" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>13.94</v>
+        <v>21</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>94.56999999999999</v>
+        <v>144.58</v>
       </c>
       <c r="I33" s="2" t="n">
         <v>4.6</v>
@@ -3570,7 +3579,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="2" t="n">
-        <v>139.17</v>
+        <v>189.18</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1" s="3">
@@ -3581,7 +3590,7 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>~{DRAM_CS1_B}</t>
+          <t>DRAM_CA3_B</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -3593,28 +3602,28 @@
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>10.63</v>
+        <v>18.26</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>11.03</v>
+        <v>18.66</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>73.95</v>
+        <v>127.99</v>
       </c>
       <c r="I34" s="2" t="n">
         <v>4.6</v>
       </c>
       <c r="J34" s="2" t="n">
-        <v>47.7</v>
+        <v>56.5</v>
       </c>
       <c r="K34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L34" s="2" t="n">
-        <v>126.25</v>
+        <v>189.09</v>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1" s="3">
@@ -3625,7 +3634,7 @@
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>DRAM_CA2_B</t>
+          <t>DRAM_CKE0_B</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -3633,32 +3642,32 @@
       </c>
       <c r="D35" s="2" t="inlineStr">
         <is>
-          <t>F.Cu, In2.Cu</t>
+          <t>F.Cu, In2.Cu, B.Cu</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>17.89</v>
+        <v>19.42</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>18.29</v>
+        <v>20.82</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>125.36</v>
+        <v>135.63</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>4.6</v>
+        <v>20.3</v>
       </c>
       <c r="J35" s="2" t="n">
-        <v>59.5</v>
+        <v>51.6</v>
       </c>
       <c r="K35" s="2" t="n">
-        <v>0</v>
+        <v>-18.48</v>
       </c>
       <c r="L35" s="2" t="n">
-        <v>189.46</v>
+        <v>189.05</v>
       </c>
     </row>
     <row r="36" ht="13.5" customHeight="1" s="3">
@@ -3739,7 +3748,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="1" sqref="A36:B36 L12"/>
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.43359375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -4323,7 +4332,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="A36:B36 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -5302,7 +5311,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A36:B36 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -5662,7 +5671,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A36:B36 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.2890625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>

<commit_message>
length matched DDR_B byte 0
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -92,15 +92,6 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -2088,7 +2079,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J42" activeCellId="0" sqref="J42"/>
+      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -2766,16 +2757,16 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>10.79</v>
+        <v>10.71</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>13.19</v>
+        <v>13.11</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>63.18</v>
+        <v>62.74</v>
       </c>
       <c r="I15" s="2" t="n">
         <v>36</v>
@@ -2787,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>147.78</v>
+        <v>147.34</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
@@ -2810,16 +2801,16 @@
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>10.59</v>
+        <v>10.73</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>12.99</v>
+        <v>13.13</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>62.05</v>
+        <v>62.83</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>36</v>
@@ -2831,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>146.65</v>
+        <v>147.43</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" s="3">
@@ -2854,16 +2845,16 @@
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>13.37</v>
+        <v>16.99</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>13.37</v>
+        <v>16.99</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>78.05</v>
+        <v>99.27</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>0</v>
@@ -2875,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>126.05</v>
+        <v>147.27</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" s="3">
@@ -2898,16 +2889,16 @@
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>11.92</v>
+        <v>16.7</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>11.92</v>
+        <v>16.7</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>69.64</v>
+        <v>97.62</v>
       </c>
       <c r="I18" s="2" t="n">
         <v>0</v>
@@ -2919,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>119.44</v>
+        <v>147.42</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" s="3">
@@ -2942,16 +2933,16 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>10.8</v>
+        <v>15.84</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>10.8</v>
+        <v>15.84</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>63.12</v>
+        <v>92.61</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>0</v>
@@ -2963,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>117.82</v>
+        <v>147.31</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
@@ -2986,16 +2977,16 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>10.95</v>
+        <v>16.05</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>10.95</v>
+        <v>16.05</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>63.86</v>
+        <v>93.73999999999999</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>0</v>
@@ -3007,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>117.46</v>
+        <v>147.34</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" s="3">
@@ -3030,16 +3021,16 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>9.289999999999999</v>
+        <v>16.17</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>9.289999999999999</v>
+        <v>16.17</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>54.26</v>
+        <v>94.58</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>0</v>
@@ -3051,7 +3042,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>107.06</v>
+        <v>147.38</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
@@ -3074,16 +3065,16 @@
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>9.42</v>
+        <v>16.38</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>9.42</v>
+        <v>16.38</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>54.93</v>
+        <v>95.67</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
@@ -3095,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>106.43</v>
+        <v>147.17</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
@@ -3118,16 +3109,16 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>8.5</v>
+        <v>15.84</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>8.5</v>
+        <v>15.84</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>49.64</v>
+        <v>92.63</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>0</v>
@@ -3139,7 +3130,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>104.14</v>
+        <v>147.13</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">
@@ -3162,16 +3153,16 @@
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>8.48</v>
+        <v>16.64</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>8.48</v>
+        <v>16.64</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>49.44</v>
+        <v>97.23</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>0</v>
@@ -3183,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>99.34</v>
+        <v>147.13</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" s="3">
@@ -3206,16 +3197,16 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>8.57</v>
+        <v>18.04</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>8.57</v>
+        <v>18.04</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>49.87</v>
+        <v>105.34</v>
       </c>
       <c r="I25" s="2" t="n">
         <v>0</v>
@@ -3227,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>91.87</v>
+        <v>147.34</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" s="3">

</xml_diff>

<commit_message>
fix some drc errors in ddr area
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -92,6 +92,15 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -2079,7 +2088,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -2261,7 +2270,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS1_B_N</t>
+          <t>DRAM_DQS1_B_P</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -2273,28 +2282,28 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>18.65</v>
+        <v>18.53</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>21.05</v>
+        <v>20.93</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>109.24</v>
+        <v>108.4</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>36</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>55</v>
+        <v>55.5</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>200.24</v>
+        <v>199.9</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="3">
@@ -2305,7 +2314,7 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS1_B_P</t>
+          <t>DRAM_DQS1_B_N</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -2317,28 +2326,28 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>18.63</v>
+        <v>18.55</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>21.03</v>
+        <v>20.95</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>108.97</v>
+        <v>108.67</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>36</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>55.5</v>
+        <v>55</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>200.47</v>
+        <v>199.67</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="3">
@@ -2713,16 +2722,16 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>21.85</v>
+        <v>21.84</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>22.25</v>
+        <v>22.24</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>150.98</v>
+        <v>150.9</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>4.6</v>
@@ -2734,7 +2743,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>199.78</v>
+        <v>199.7</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="3">
@@ -2745,7 +2754,7 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS0_B_N</t>
+          <t>DRAM_DQS0_B_P</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -2757,16 +2766,16 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>10.71</v>
+        <v>10.73</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>13.11</v>
+        <v>13.13</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>62.74</v>
+        <v>62.83</v>
       </c>
       <c r="I15" s="2" t="n">
         <v>36</v>
@@ -2778,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>147.34</v>
+        <v>147.43</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" s="3">
@@ -2789,7 +2798,7 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DQS0_B_P</t>
+          <t>DRAM_DQS0_B_N</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -2801,16 +2810,16 @@
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>10.73</v>
+        <v>10.71</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>13.13</v>
+        <v>13.11</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>62.83</v>
+        <v>62.74</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>36</v>
@@ -2822,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>147.43</v>
+        <v>147.34</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" s="3">
@@ -2833,7 +2842,7 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D07_B</t>
+          <t>DRAM_D05_B</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -2845,28 +2854,28 @@
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>16.99</v>
+        <v>16.7</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>16.99</v>
+        <v>16.7</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>99.27</v>
+        <v>97.62</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>48</v>
+        <v>49.8</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>147.27</v>
+        <v>147.42</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" s="3">
@@ -2877,7 +2886,7 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D05_B</t>
+          <t>DRAM_DMI0_B</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -2889,28 +2898,28 @@
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>16.7</v>
+        <v>16.17</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>16.7</v>
+        <v>16.17</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>97.62</v>
+        <v>94.58</v>
       </c>
       <c r="I18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>49.8</v>
+        <v>52.8</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>147.42</v>
+        <v>147.38</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" s="3">
@@ -2921,7 +2930,7 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D06_B</t>
+          <t>DRAM_D04_B</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -2933,28 +2942,28 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>15.84</v>
+        <v>16.05</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>15.84</v>
+        <v>16.05</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>92.61</v>
+        <v>93.73999999999999</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>54.7</v>
+        <v>53.6</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>147.31</v>
+        <v>147.34</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
@@ -2965,7 +2974,7 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D04_B</t>
+          <t>DRAM_D03_B</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -2977,22 +2986,22 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>16.05</v>
+        <v>18.04</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>16.05</v>
+        <v>18.04</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>93.73999999999999</v>
+        <v>105.34</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>53.6</v>
+        <v>42</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>0</v>
@@ -3009,7 +3018,7 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>DRAM_DMI0_B</t>
+          <t>DRAM_D06_B</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -3021,28 +3030,28 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>16.17</v>
+        <v>15.84</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>16.17</v>
+        <v>15.84</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>94.58</v>
+        <v>92.61</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>52.8</v>
+        <v>54.7</v>
       </c>
       <c r="K21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>147.38</v>
+        <v>147.31</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
@@ -3053,7 +3062,7 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D00_B</t>
+          <t>DRAM_D07_B</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -3065,28 +3074,28 @@
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>16.38</v>
+        <v>16.99</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>16.38</v>
+        <v>16.99</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>95.67</v>
+        <v>99.27</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>51.5</v>
+        <v>48</v>
       </c>
       <c r="K22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>147.17</v>
+        <v>147.27</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
@@ -3097,7 +3106,7 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D02_B</t>
+          <t>DRAM_D00_B</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -3109,28 +3118,28 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>15.84</v>
+        <v>16.41</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>15.84</v>
+        <v>16.41</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>92.63</v>
+        <v>95.87</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>54.5</v>
+        <v>51.5</v>
       </c>
       <c r="K23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>147.13</v>
+        <v>147.37</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">
@@ -3141,7 +3150,7 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D01_B</t>
+          <t>DRAM_D02_B</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -3153,22 +3162,22 @@
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>16.64</v>
+        <v>15.84</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>16.64</v>
+        <v>15.84</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>97.23</v>
+        <v>92.63</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="2" t="n">
-        <v>49.9</v>
+        <v>54.5</v>
       </c>
       <c r="K24" s="2" t="n">
         <v>0</v>
@@ -3185,7 +3194,7 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D03_B</t>
+          <t>DRAM_D01_B</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -3197,28 +3206,28 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>18.04</v>
+        <v>16.64</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>18.04</v>
+        <v>16.64</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>105.34</v>
+        <v>97.23</v>
       </c>
       <c r="I25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="2" t="n">
-        <v>42</v>
+        <v>49.9</v>
       </c>
       <c r="K25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>147.34</v>
+        <v>147.13</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" s="3">

</xml_diff>

<commit_message>
bom work, change uart level shifter and m.2 socket
</commit_message>
<xml_diff>
--- a/flytimes.xlsx
+++ b/flytimes.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DDR_A" sheetId="1" state="visible" r:id="rId1"/>
@@ -92,15 +92,6 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -463,8 +454,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -1230,16 +1221,16 @@
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>20.84</v>
+        <v>20.79</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>21.24</v>
+        <v>21.19</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>142</v>
+        <v>141.82</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>4.6</v>
@@ -1251,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>198</v>
+        <v>197.82</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" s="3">
@@ -1274,16 +1265,16 @@
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>20.52</v>
+        <v>20.49</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>20.92</v>
+        <v>20.89</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>141.7</v>
+        <v>141.53</v>
       </c>
       <c r="I18" s="2" t="n">
         <v>4.6</v>
@@ -1295,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>198</v>
+        <v>197.83</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" s="3">
@@ -1318,16 +1309,16 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>19.82</v>
+        <v>19.55</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>20.22</v>
+        <v>19.95</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>136.17</v>
+        <v>136.06</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>4.6</v>
@@ -1339,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>197.97</v>
+        <v>197.86</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
@@ -1406,16 +1397,16 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>22.79</v>
+        <v>22.23</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>23.19</v>
+        <v>22.63</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>150.29</v>
+        <v>150.31</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>4.6</v>
@@ -1427,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>197.89</v>
+        <v>197.91</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
@@ -1494,16 +1485,16 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>18.88</v>
+        <v>18.87</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>19.28</v>
+        <v>19.27</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>128.6</v>
+        <v>128.51</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>4.6</v>
@@ -1515,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>197.8</v>
+        <v>197.71</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">
@@ -1538,16 +1529,16 @@
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>21.89</v>
+        <v>21.82</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>22.29</v>
+        <v>22.22</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>150.43</v>
+        <v>150.56</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>4.6</v>
@@ -1559,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>197.73</v>
+        <v>197.86</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" s="3">
@@ -1582,16 +1573,16 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>20.04</v>
+        <v>20.07</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>20.44</v>
+        <v>20.47</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>138.45</v>
+        <v>138.63</v>
       </c>
       <c r="I25" s="2" t="n">
         <v>4.6</v>
@@ -1603,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>197.65</v>
+        <v>197.83</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" s="3">
@@ -2087,8 +2078,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -2930,7 +2921,7 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D04_B</t>
+          <t>DRAM_D00_B</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -2942,28 +2933,28 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>16.05</v>
+        <v>16.41</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>16.05</v>
+        <v>16.41</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>93.73999999999999</v>
+        <v>95.87</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>53.6</v>
+        <v>51.5</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>147.34</v>
+        <v>147.37</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" s="3">
@@ -2974,7 +2965,7 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D03_B</t>
+          <t>DRAM_D04_B</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -2986,22 +2977,22 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>18.04</v>
+        <v>16.05</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>18.04</v>
+        <v>16.05</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>105.34</v>
+        <v>93.73999999999999</v>
       </c>
       <c r="I20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>42</v>
+        <v>53.6</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>0</v>
@@ -3018,7 +3009,7 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D06_B</t>
+          <t>DRAM_D03_B</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -3030,28 +3021,28 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>15.84</v>
+        <v>18.04</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>15.84</v>
+        <v>18.04</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>92.61</v>
+        <v>105.34</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>54.7</v>
+        <v>42</v>
       </c>
       <c r="K21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>147.31</v>
+        <v>147.34</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" s="3">
@@ -3062,7 +3053,7 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D07_B</t>
+          <t>DRAM_D06_B</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -3074,28 +3065,28 @@
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>16.99</v>
+        <v>15.84</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>16.99</v>
+        <v>15.84</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>99.27</v>
+        <v>92.61</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>48</v>
+        <v>54.7</v>
       </c>
       <c r="K22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>147.27</v>
+        <v>147.31</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="3">
@@ -3106,7 +3097,7 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>DRAM_D00_B</t>
+          <t>DRAM_D07_B</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -3118,28 +3109,28 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>16.41</v>
+        <v>16.99</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>16.41</v>
+        <v>16.99</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>95.87</v>
+        <v>99.27</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>51.5</v>
+        <v>48</v>
       </c>
       <c r="K23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>147.37</v>
+        <v>147.27</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" s="3">

</xml_diff>